<commit_message>
graph change 2 + testing different configs + performance boost
</commit_message>
<xml_diff>
--- a/flow_config.xlsx
+++ b/flow_config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="flow_matrix"/>
@@ -20,31 +20,31 @@
     <t>extremity_id</t>
   </si>
   <si>
-    <t>spawn_interval</t>
-  </si>
-  <si>
-    <t>spawner_0</t>
-  </si>
-  <si>
-    <t>spawner_1</t>
-  </si>
-  <si>
-    <t>spawner_2</t>
-  </si>
-  <si>
-    <t>spawner_3</t>
-  </si>
-  <si>
-    <t>spawner_4</t>
-  </si>
-  <si>
-    <t>spawner_5</t>
-  </si>
-  <si>
-    <t>spawner_6</t>
-  </si>
-  <si>
-    <t>spawner_7</t>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>sp0</t>
+  </si>
+  <si>
+    <t>sp1</t>
+  </si>
+  <si>
+    <t>sp2</t>
+  </si>
+  <si>
+    <t>sp3</t>
+  </si>
+  <si>
+    <t>sp4</t>
+  </si>
+  <si>
+    <t>sp5</t>
+  </si>
+  <si>
+    <t>sp6</t>
+  </si>
+  <si>
+    <t>sp7</t>
   </si>
 </sst>
 </file>
@@ -62,7 +62,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -123,7 +123,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -132,13 +132,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -448,7 +448,7 @@
   </sheetPr>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -463,7 +463,7 @@
     <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>2</v>
@@ -490,7 +490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -519,7 +519,7 @@
         <v>0.1428571428571428</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -548,7 +548,7 @@
         <v>0.1428571428571428</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -577,7 +577,7 @@
         <v>0.1428571428571428</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -606,7 +606,7 @@
         <v>0.1428571428571428</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -635,7 +635,7 @@
         <v>0.1428571428571428</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -664,7 +664,7 @@
         <v>0.1428571428571428</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0.1428571428571428</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -734,7 +734,7 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>